<commit_message>
Calcul un pourcentage de certitude de durée de note
Calcul la probabilité qu'un segment appartienne à un certaine classe de durée de note.
Pour l'instant cette probabilité est exploitée à Minima puisqu'on ne garde que la classe de la meilleure certitude.
Les probabilités ont été changées pour avoir de meilleur résultat (apprentissage à la main).
</commit_message>
<xml_diff>
--- a/Docs/Résultats_21_10_15.xlsx
+++ b/Docs/Résultats_21_10_15.xlsx
@@ -403,7 +403,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,15 +465,15 @@
       <c r="D2">
         <v>8</v>
       </c>
-      <c r="E2">
-        <v>4.7618999999999998</v>
-      </c>
-      <c r="F2">
-        <v>9.5237999999999996</v>
-      </c>
-      <c r="G2">
-        <f>100-E2-F2</f>
-        <v>85.714300000000009</v>
+      <c r="E2" s="2">
+        <v>4.7619000000000002E-2</v>
+      </c>
+      <c r="F2" s="2">
+        <v>9.5238000000000003E-2</v>
+      </c>
+      <c r="G2" s="2">
+        <f>100%-(E2)-(F2)</f>
+        <v>0.85714299999999999</v>
       </c>
       <c r="H2" s="2">
         <v>0.64705900000000005</v>
@@ -501,15 +501,15 @@
       <c r="D3">
         <v>8</v>
       </c>
-      <c r="E3">
-        <v>12.5</v>
-      </c>
-      <c r="F3">
+      <c r="E3" s="2">
+        <v>0.125</v>
+      </c>
+      <c r="F3" s="3">
         <v>0</v>
       </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G6" si="0">100-E3-F3</f>
-        <v>87.5</v>
+      <c r="G3" s="2">
+        <f t="shared" ref="G3:G6" si="0">100%-(E3)-(F3)</f>
+        <v>0.875</v>
       </c>
       <c r="H3" s="3">
         <v>1</v>
@@ -537,15 +537,15 @@
       <c r="D4">
         <v>16</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3">
         <v>0</v>
       </c>
-      <c r="F4">
-        <v>7.8947000000000003</v>
-      </c>
-      <c r="G4">
+      <c r="F4" s="2">
+        <v>7.8947000000000003E-2</v>
+      </c>
+      <c r="G4" s="2">
         <f t="shared" si="0"/>
-        <v>92.1053</v>
+        <v>0.92105300000000001</v>
       </c>
       <c r="H4" s="3">
         <v>1</v>
@@ -573,15 +573,15 @@
       <c r="D5">
         <v>30</v>
       </c>
-      <c r="E5">
-        <v>4.2553000000000001</v>
-      </c>
-      <c r="F5">
-        <v>34.0426</v>
-      </c>
-      <c r="G5">
+      <c r="E5" s="2">
+        <v>4.2553000000000001E-2</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.34042600000000001</v>
+      </c>
+      <c r="G5" s="2">
         <f t="shared" si="0"/>
-        <v>61.702099999999994</v>
+        <v>0.61702100000000004</v>
       </c>
       <c r="H5" s="2">
         <v>0.85294000000000003</v>
@@ -609,15 +609,15 @@
       <c r="D6">
         <v>35</v>
       </c>
-      <c r="E6">
-        <v>14.2857</v>
-      </c>
-      <c r="F6">
-        <v>8.7911999999999999</v>
-      </c>
-      <c r="G6">
+      <c r="E6" s="2">
+        <v>0.14285700000000001</v>
+      </c>
+      <c r="F6" s="2">
+        <v>8.7912000000000004E-2</v>
+      </c>
+      <c r="G6" s="2">
         <f t="shared" si="0"/>
-        <v>76.923099999999991</v>
+        <v>0.769231</v>
       </c>
       <c r="H6" s="3">
         <v>0.75</v>
@@ -634,5 +634,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>